<commit_message>
Interviewskills added in stackraking script
</commit_message>
<xml_diff>
--- a/Input Data/Crpo/stackranking/stack_ranking_FourEvents_report.xlsx
+++ b/Input Data/Crpo/stackranking/stack_ranking_FourEvents_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="40">
   <si>
     <t>Applicant Id</t>
   </si>
@@ -94,12 +94,21 @@
     <t>HRM General Knowledge</t>
   </si>
   <si>
+    <t>42833</t>
+  </si>
+  <si>
+    <t>42834</t>
+  </si>
+  <si>
+    <t>42835</t>
+  </si>
+  <si>
+    <t>HRMM GK Automobile Engineering</t>
+  </si>
+  <si>
     <t>Coding Assessment</t>
   </si>
   <si>
-    <t>HRMM GK Automobile Engineering</t>
-  </si>
-  <si>
     <t>Stack Ranking One</t>
   </si>
   <si>
@@ -112,10 +121,10 @@
     <t>Not Specified</t>
   </si>
   <si>
-    <t>Assessment</t>
-  </si>
-  <si>
-    <t>Pending</t>
+    <t>First Interview</t>
+  </si>
+  <si>
+    <t>Shortlisted</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -521,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AU7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -534,7 +543,7 @@
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" customWidth="1"/>
@@ -562,9 +571,21 @@
     <col min="33" max="33" width="12.7109375" customWidth="1"/>
     <col min="34" max="34" width="7.7109375" customWidth="1"/>
     <col min="35" max="35" width="10.7109375" customWidth="1"/>
+    <col min="36" max="36" width="11.7109375" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="38" max="38" width="7.7109375" customWidth="1"/>
+    <col min="39" max="39" width="10.7109375" customWidth="1"/>
+    <col min="40" max="40" width="11.7109375" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" customWidth="1"/>
+    <col min="42" max="42" width="7.7109375" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" customWidth="1"/>
+    <col min="44" max="44" width="11.7109375" customWidth="1"/>
+    <col min="45" max="45" width="12.7109375" customWidth="1"/>
+    <col min="46" max="46" width="7.7109375" customWidth="1"/>
+    <col min="47" max="47" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:47">
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
@@ -583,8 +604,20 @@
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:47">
       <c r="T2" s="1" t="s">
         <v>24</v>
       </c>
@@ -609,8 +642,26 @@
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
+      <c r="AJ2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:47">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,8 +767,44 @@
       <c r="AI3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="AJ3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:47">
       <c r="A4" s="2">
         <v>896910</v>
       </c>
@@ -725,61 +812,61 @@
         <v>1290157</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G4" s="3">
         <v>33992</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="S4" s="2">
-        <v>44.75</v>
+        <v>46.38</v>
       </c>
       <c r="T4" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="U4" s="2">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V4" s="2">
         <v>7</v>
@@ -788,10 +875,10 @@
         <v>10</v>
       </c>
       <c r="X4" s="2">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="Y4" s="2">
-        <v>23.75</v>
+        <v>14.25</v>
       </c>
       <c r="Z4" s="2">
         <v>19</v>
@@ -799,246 +886,354 @@
       <c r="AA4" s="2">
         <v>20</v>
       </c>
-      <c r="AB4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>34</v>
+      <c r="AB4" s="2">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>25</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>50</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>11.25</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>60</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ4" s="2">
+        <v>5</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>1.88</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>8</v>
+      </c>
+      <c r="AN4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AU4" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:47">
       <c r="A5" s="2">
-        <v>896909</v>
+        <v>896911</v>
       </c>
       <c r="B5" s="2">
         <v>1290157</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G5" s="3">
         <v>33992</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="2">
+        <v>44.51</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>10</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>7</v>
+      </c>
+      <c r="AD5" s="2">
         <v>35</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="2">
-        <v>36</v>
-      </c>
-      <c r="T5" s="2">
+      <c r="AE5" s="2">
+        <v>50</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>15</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>9.38</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>50</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>5</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>3.13</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>5</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>8</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>25</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>25</v>
+      </c>
+      <c r="AP5" s="2">
         <v>30</v>
       </c>
-      <c r="U5" s="2">
-        <v>22.5</v>
-      </c>
-      <c r="V5" s="2">
-        <v>15</v>
-      </c>
-      <c r="W5" s="2">
-        <v>20</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>15</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>13.5</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>9</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI5" s="4" t="s">
-        <v>34</v>
+      <c r="AQ5" s="2">
+        <v>30</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:47">
       <c r="A6" s="2">
-        <v>896911</v>
+        <v>896909</v>
       </c>
       <c r="B6" s="2">
         <v>1290157</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G6" s="3">
         <v>33992</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" s="2">
+        <v>43.51</v>
+      </c>
+      <c r="T6" s="2">
+        <v>20</v>
+      </c>
+      <c r="U6" s="2">
+        <v>15</v>
+      </c>
+      <c r="V6" s="2">
+        <v>15</v>
+      </c>
+      <c r="W6" s="2">
+        <v>20</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>10</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>7</v>
+      </c>
+      <c r="AD6" s="2">
         <v>35</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" s="2">
-        <v>30</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="V6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE6" s="4" t="s">
-        <v>34</v>
+      <c r="AE6" s="2">
+        <v>50</v>
       </c>
       <c r="AF6" s="2">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AG6" s="2">
-        <v>30</v>
+        <v>9.38</v>
       </c>
       <c r="AH6" s="2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="AI6" s="2">
-        <v>30</v>
+        <v>80</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>5</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>3.13</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>5</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>8</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>10</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>9</v>
+      </c>
+      <c r="AT6" s="2">
+        <v>9</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:47">
       <c r="A7" s="2">
         <v>896908</v>
       </c>
@@ -1046,61 +1241,61 @@
         <v>1290157</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G7" s="3">
         <v>33992</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="S7" s="2">
-        <v>18</v>
+        <v>31.01</v>
       </c>
       <c r="T7" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="U7" s="2">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="V7" s="2">
         <v>18</v>
@@ -1109,49 +1304,88 @@
         <v>30</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI7" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>10</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>50</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>15</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>5.63</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>30</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>7</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>8</v>
+      </c>
+      <c r="AN7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AU7" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="T1:AI1"/>
+  <mergeCells count="8">
+    <mergeCell ref="T1:AU1"/>
     <mergeCell ref="T2:W2"/>
     <mergeCell ref="X2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="AF2:AI2"/>
+    <mergeCell ref="AJ2:AM2"/>
+    <mergeCell ref="AN2:AQ2"/>
+    <mergeCell ref="AR2:AU2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>